<commit_message>
Prepare interview outline & papers 3 and 4
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Tesi\KIT-VR_and_accessibility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2C6281-A5A2-4084-A9F7-0CB0735AE40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B56288-E914-49BC-954C-83DC0D8778C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{09907DBE-A90C-4710-9E50-F780C15D1BDC}"/>
   </bookViews>
@@ -96,13 +96,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,7 +441,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,14 +458,14 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="1"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="2"/>
+      <c r="I3" s="3"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -478,41 +478,41 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -525,19 +525,19 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -569,15 +569,15 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -588,7 +588,7 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>

</xml_diff>